<commit_message>
Polishing cleaning documentation #1
</commit_message>
<xml_diff>
--- a/csv files/stations/trips_p1_stations.xlsx
+++ b/csv files/stations/trips_p1_stations.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\divvy-bikeshare\csv files\stations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EA145472-17AC-4B58-811B-6F2E1A2DA545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E484F6-ED90-48D5-B01F-42FC1FADCFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13095" yWindow="555" windowWidth="12120" windowHeight="14445"/>
+    <workbookView xWindow="-12870" yWindow="1110" windowWidth="10905" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trips_p1_stations" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,23 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Stations!$A$1:$H$1291</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">trips_p1_stations!$A$1:$E$150</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Query - Stations" description="Connection to the 'Stations' query in the workbook." type="5" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - Stations" description="Connection to the 'Stations' query in the workbook." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Stations;Extended Properties=&quot;&quot;" command="SELECT * FROM [Stations]"/>
   </connection>
 </connections>
@@ -19817,7 +19827,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -20343,47 +20353,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -20441,206 +20411,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -20963,13 +20733,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20999,10 +20768,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B2,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21010,19 +20779,19 @@
       </c>
       <c r="D2" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A2,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>900 W Harrison St</v>
+        <v>same</v>
       </c>
       <c r="E2" t="str">
         <f>IF(AND(D2="same",C2="same"),"missing",IF(B2=D2,"same",IF(AND(A2&lt;&gt;C2,D2="same"),"id",IF(B2&lt;&gt;D2,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C3" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B3,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21030,7 +20799,7 @@
       </c>
       <c r="D3" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A3,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Aberdeen St &amp; Monroe St</v>
+        <v>Buckingham Fountain</v>
       </c>
       <c r="E3" t="str">
         <f>IF(AND(D3="same",C3="same"),"missing",IF(B3=D3,"same",IF(AND(A3&lt;&gt;C3,D3="same"),"id",IF(B3&lt;&gt;D3,"name"))))</f>
@@ -21039,10 +20808,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B4,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21050,7 +20819,7 @@
       </c>
       <c r="D4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A4,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Aberdeen St &amp; Monroe St</v>
+        <v>Paulina Ave &amp; North Ave</v>
       </c>
       <c r="E4" t="str">
         <f>IF(AND(D4="same",C4="same"),"missing",IF(B4=D4,"same",IF(AND(A4&lt;&gt;C4,D4="same"),"id",IF(B4&lt;&gt;D4,"name"))))</f>
@@ -21059,10 +20828,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>480</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B5,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21070,7 +20839,7 @@
       </c>
       <c r="D5" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A5,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Albany Ave &amp; Montrose Ave</v>
+        <v>Paulina Ave &amp; North Ave</v>
       </c>
       <c r="E5" t="str">
         <f>IF(AND(D5="same",C5="same"),"missing",IF(B5=D5,"same",IF(AND(A5&lt;&gt;C5,D5="same"),"id",IF(B5&lt;&gt;D5,"name"))))</f>
@@ -21079,10 +20848,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>645</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>8</v>
       </c>
       <c r="C6" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B6,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21090,7 +20859,7 @@
       </c>
       <c r="D6" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A6,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Archer Damen Ave &amp; 37th St</v>
+        <v>Honore St &amp; Division St</v>
       </c>
       <c r="E6" t="str">
         <f>IF(AND(D6="same",C6="same"),"missing",IF(B6=D6,"same",IF(AND(A6&lt;&gt;C6,D6="same"),"id",IF(B6&lt;&gt;D6,"name"))))</f>
@@ -21099,10 +20868,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>208</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B7,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21110,7 +20879,7 @@
       </c>
       <c r="D7" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A7,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Laflin St &amp; Cullerton St</v>
+        <v>Throop St &amp; Taylor St</v>
       </c>
       <c r="E7" t="str">
         <f>IF(AND(D7="same",C7="same"),"missing",IF(B7=D7,"same",IF(AND(A7&lt;&gt;C7,D7="same"),"id",IF(B7&lt;&gt;D7,"name"))))</f>
@@ -21119,10 +20888,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>566</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B8,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21130,7 +20899,7 @@
       </c>
       <c r="D8" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A8,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Damen Ave &amp; 74th St</v>
+        <v>Throop St &amp; Taylor St</v>
       </c>
       <c r="E8" t="str">
         <f>IF(AND(D8="same",C8="same"),"missing",IF(B8=D8,"same",IF(AND(A8&lt;&gt;C8,D8="same"),"id",IF(B8&lt;&gt;D8,"name"))))</f>
@@ -21139,10 +20908,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>383</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B9,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21150,7 +20919,7 @@
       </c>
       <c r="D9" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A9,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Paulina St &amp; Flournoy St</v>
+        <v>Throop St &amp; Taylor St</v>
       </c>
       <c r="E9" t="str">
         <f>IF(AND(D9="same",C9="same"),"missing",IF(B9=D9,"same",IF(AND(A9&lt;&gt;C9,D9="same"),"id",IF(B9&lt;&gt;D9,"name"))))</f>
@@ -21159,10 +20928,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>119</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C10" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B10,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21170,19 +20939,19 @@
       </c>
       <c r="D10" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A10,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Ashland Ave &amp; Lake St</v>
+        <v>Orleans St &amp; Elm St</v>
       </c>
       <c r="E10" t="str">
         <f>IF(AND(D10="same",C10="same"),"missing",IF(B10=D10,"same",IF(AND(A10&lt;&gt;C10,D10="same"),"id",IF(B10&lt;&gt;D10,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>512</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B11,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21190,19 +20959,19 @@
       </c>
       <c r="D11" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A11,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>New St &amp; Illinois St</v>
       </c>
       <c r="E11" t="str">
         <f>IF(AND(D11="same",C11="same"),"missing",IF(B11=D11,"same",IF(AND(A11&lt;&gt;C11,D11="same"),"id",IF(B11&lt;&gt;D11,"name"))))</f>
-        <v>missing</v>
+        <v>name</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>293</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B12,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21210,7 +20979,7 @@
       </c>
       <c r="D12" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A12,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Broadway &amp; Wilson - Truman College Vaccination Site</v>
+        <v>Franklin St &amp; Chicago Ave</v>
       </c>
       <c r="E12" t="str">
         <f>IF(AND(D12="same",C12="same"),"missing",IF(B12=D12,"same",IF(AND(A12&lt;&gt;C12,D12="same"),"id",IF(B12&lt;&gt;D12,"name"))))</f>
@@ -21219,10 +20988,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>332</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B13,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21230,19 +20999,19 @@
       </c>
       <c r="D13" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A13,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Burling St &amp; Diversey Pkwy</v>
+        <v>Streeter Dr &amp; Grand Ave</v>
       </c>
       <c r="E13" t="str">
         <f>IF(AND(D13="same",C13="same"),"missing",IF(B13=D13,"same",IF(AND(A13&lt;&gt;C13,D13="same"),"id",IF(B13&lt;&gt;D13,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>372</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="C14" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B14,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21250,19 +21019,19 @@
       </c>
       <c r="D14" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A14,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Michigan Ave &amp; Ida B Wells Dr</v>
       </c>
       <c r="E14" t="str">
         <f>IF(AND(D14="same",C14="same"),"missing",IF(B14=D14,"same",IF(AND(A14&lt;&gt;C14,D14="same"),"id",IF(B14&lt;&gt;D14,"name"))))</f>
-        <v>missing</v>
+        <v>name</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>259</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="C15" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B15,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21270,7 +21039,7 @@
       </c>
       <c r="D15" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A15,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>California Ave &amp; Francis Pl Temp</v>
+        <v>Clark St &amp; Ida B Wells Dr</v>
       </c>
       <c r="E15" t="str">
         <f>IF(AND(D15="same",C15="same"),"missing",IF(B15=D15,"same",IF(AND(A15&lt;&gt;C15,D15="same"),"id",IF(B15&lt;&gt;D15,"name"))))</f>
@@ -21279,10 +21048,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>436</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
       <c r="C16" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B16,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21290,7 +21059,7 @@
       </c>
       <c r="D16" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A16,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Fairfield Ave &amp; Roosevelt Rd</v>
+        <v>Wells St &amp; Huron St</v>
       </c>
       <c r="E16" t="str">
         <f>IF(AND(D16="same",C16="same"),"missing",IF(B16=D16,"same",IF(AND(A16&lt;&gt;C16,D16="same"),"id",IF(B16&lt;&gt;D16,"name"))))</f>
@@ -21299,10 +21068,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>191</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B17,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21310,7 +21079,7 @@
       </c>
       <c r="D17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A17,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Canal St &amp; Monroe St</v>
+        <v>Wells St &amp; Huron St</v>
       </c>
       <c r="E17" t="str">
         <f>IF(AND(D17="same",C17="same"),"missing",IF(B17=D17,"same",IF(AND(A17&lt;&gt;C17,D17="same"),"id",IF(B17&lt;&gt;D17,"name"))))</f>
@@ -21319,10 +21088,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>578</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>20</v>
       </c>
       <c r="C18" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B18,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21330,7 +21099,7 @@
       </c>
       <c r="D18" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A18,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Bennett Ave &amp; 79th St</v>
+        <v>Halsted St &amp; Roosevelt Rd</v>
       </c>
       <c r="E18" t="str">
         <f>IF(AND(D18="same",C18="same"),"missing",IF(B18=D18,"same",IF(AND(A18&lt;&gt;C18,D18="same"),"id",IF(B18&lt;&gt;D18,"name"))))</f>
@@ -21339,10 +21108,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>625</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
       <c r="C19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B19,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21350,7 +21119,7 @@
       </c>
       <c r="D19" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A19,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Dodge Ave &amp; Main St</v>
+        <v>Elston Ave &amp; Cortland St</v>
       </c>
       <c r="E19" t="str">
         <f>IF(AND(D19="same",C19="same"),"missing",IF(B19=D19,"same",IF(AND(A19&lt;&gt;C19,D19="same"),"id",IF(B19&lt;&gt;D19,"name"))))</f>
@@ -21359,10 +21128,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C20" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B20,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21370,7 +21139,7 @@
       </c>
       <c r="D20" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A20,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Clark St &amp; Ida B Wells Dr</v>
+        <v>Wabash Ave &amp; 16th St</v>
       </c>
       <c r="E20" t="str">
         <f>IF(AND(D20="same",C20="same"),"missing",IF(B20=D20,"same",IF(AND(A20&lt;&gt;C20,D20="same"),"id",IF(B20&lt;&gt;D20,"name"))))</f>
@@ -21379,10 +21148,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>325</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="C21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B21,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21390,7 +21159,7 @@
       </c>
       <c r="D21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A21,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Clark St &amp; Winnemac Ave</v>
+        <v>Wabash Ave &amp; 16th St</v>
       </c>
       <c r="E21" t="str">
         <f>IF(AND(D21="same",C21="same"),"missing",IF(B21=D21,"same",IF(AND(A21&lt;&gt;C21,D21="same"),"id",IF(B21&lt;&gt;D21,"name"))))</f>
@@ -21399,10 +21168,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>253</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C22" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B22,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21410,7 +21179,7 @@
       </c>
       <c r="D22" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A22,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Winthrop Ave &amp; Lawrence Ave</v>
+        <v>DuSable Lake Shore Dr &amp; Monroe St</v>
       </c>
       <c r="E22" t="str">
         <f>IF(AND(D22="same",C22="same"),"missing",IF(B22=D22,"same",IF(AND(A22&lt;&gt;C22,D22="same"),"id",IF(B22&lt;&gt;D22,"name"))))</f>
@@ -21419,10 +21188,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>638</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>25</v>
       </c>
       <c r="C23" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B23,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21430,7 +21199,7 @@
       </c>
       <c r="D23" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A23,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Clinton St &amp; Jackson Blvd</v>
+        <v>Aberdeen St &amp; Monroe St</v>
       </c>
       <c r="E23" t="str">
         <f>IF(AND(D23="same",C23="same"),"missing",IF(B23=D23,"same",IF(AND(A23&lt;&gt;C23,D23="same"),"id",IF(B23&lt;&gt;D23,"name"))))</f>
@@ -21439,10 +21208,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C24" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B24,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21450,7 +21219,7 @@
       </c>
       <c r="D24" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A24,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Clinton St &amp; Polk St</v>
+        <v>Aberdeen St &amp; Monroe St</v>
       </c>
       <c r="E24" t="str">
         <f>IF(AND(D24="same",C24="same"),"missing",IF(B24=D24,"same",IF(AND(A24&lt;&gt;C24,D24="same"),"id",IF(B24&lt;&gt;D24,"name"))))</f>
@@ -21459,10 +21228,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>417</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="C25" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B25,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21470,19 +21239,19 @@
       </c>
       <c r="D25" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A25,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Cornell Ave &amp; Hyde Park Blvd</v>
+        <v>Milwaukee Ave &amp; Grand Ave</v>
       </c>
       <c r="E25" t="str">
         <f>IF(AND(D25="same",C25="same"),"missing",IF(B25=D25,"same",IF(AND(A25&lt;&gt;C25,D25="same"),"id",IF(B25&lt;&gt;D25,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>607</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="C26" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B26,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21490,19 +21259,19 @@
       </c>
       <c r="D26" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A26,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Racine Ave &amp; Randolph St</v>
       </c>
       <c r="E26" t="str">
         <f>IF(AND(D26="same",C26="same"),"missing",IF(B26=D26,"same",IF(AND(A26&lt;&gt;C26,D26="same"),"id",IF(B26&lt;&gt;D26,"name"))))</f>
-        <v>missing</v>
+        <v>name</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>561</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
       <c r="C27" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B27,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21510,7 +21279,7 @@
       </c>
       <c r="D27" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A27,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Damen Ave &amp; 59th St</v>
+        <v>Financial Pl &amp; Ida B Wells Dr</v>
       </c>
       <c r="E27" t="str">
         <f>IF(AND(D27="same",C27="same"),"missing",IF(B27=D27,"same",IF(AND(A27&lt;&gt;C27,D27="same"),"id",IF(B27&lt;&gt;D27,"name"))))</f>
@@ -21519,10 +21288,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>183</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C28" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B28,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21530,7 +21299,7 @@
       </c>
       <c r="D28" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A28,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Damen Ave &amp; Thomas St Augusta Blvd</v>
+        <v>Financial Pl &amp; Ida B Wells Dr</v>
       </c>
       <c r="E28" t="str">
         <f>IF(AND(D28="same",C28="same"),"missing",IF(B28=D28,"same",IF(AND(A28&lt;&gt;C28,D28="same"),"id",IF(B28&lt;&gt;D28,"name"))))</f>
@@ -21539,10 +21308,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>557</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="C29" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B29,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21550,7 +21319,7 @@
       </c>
       <c r="D29" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A29,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Seeley Ave &amp; Garfield Blvd</v>
+        <v>Financial Pl &amp; Ida B Wells Dr</v>
       </c>
       <c r="E29" t="str">
         <f>IF(AND(D29="same",C29="same"),"missing",IF(B29=D29,"same",IF(AND(A29&lt;&gt;C29,D29="same"),"id",IF(B29&lt;&gt;D29,"name"))))</f>
@@ -21559,10 +21328,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>656</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>148</v>
+        <v>32</v>
       </c>
       <c r="C30" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B30,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21570,7 +21339,7 @@
       </c>
       <c r="D30" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A30,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Damen Ave &amp; Walnut Lake St</v>
+        <v>Field Museum</v>
       </c>
       <c r="E30" t="str">
         <f>IF(AND(D30="same",C30="same"),"missing",IF(B30=D30,"same",IF(AND(A30&lt;&gt;C30,D30="same"),"id",IF(B30&lt;&gt;D30,"name"))))</f>
@@ -21579,10 +21348,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>624</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
       <c r="C31" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B31,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21590,19 +21359,19 @@
       </c>
       <c r="D31" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A31,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Dearborn St &amp; Van Buren St</v>
+        <v>McClurg Ct &amp; Ohio St</v>
       </c>
       <c r="E31" t="str">
         <f>IF(AND(D31="same",C31="same"),"missing",IF(B31=D31,"same",IF(AND(A31&lt;&gt;C31,D31="same"),"id",IF(B31&lt;&gt;D31,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>361</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="C32" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B32,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21610,19 +21379,19 @@
       </c>
       <c r="D32" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A32,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Clinton St &amp; Polk St</v>
       </c>
       <c r="E32" t="str">
         <f>IF(AND(D32="same",C32="same"),"missing",IF(B32=D32,"same",IF(AND(A32&lt;&gt;C32,D32="same"),"id",IF(B32&lt;&gt;D32,"name"))))</f>
-        <v>missing</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>name</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>360</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="C33" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B33,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21630,19 +21399,19 @@
       </c>
       <c r="D33" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A33,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>900 W Harrison St</v>
       </c>
       <c r="E33" t="str">
         <f>IF(AND(D33="same",C33="same"),"missing",IF(B33=D33,"same",IF(AND(A33&lt;&gt;C33,D33="same"),"id",IF(B33&lt;&gt;D33,"name"))))</f>
-        <v>missing</v>
+        <v>name</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>503</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
       <c r="C34" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B34,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21650,19 +21419,19 @@
       </c>
       <c r="D34" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A34,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>St. Louis Ave &amp; Fullerton Ave</v>
+        <v>Dearborn St &amp; Erie St</v>
       </c>
       <c r="E34" t="str">
         <f>IF(AND(D34="same",C34="same"),"missing",IF(B34=D34,"same",IF(AND(A34&lt;&gt;C34,D34="same"),"id",IF(B34&lt;&gt;D34,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>617</v>
+        <v>114</v>
       </c>
       <c r="B35" t="s">
-        <v>131</v>
+        <v>37</v>
       </c>
       <c r="C35" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B35,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21670,19 +21439,19 @@
       </c>
       <c r="D35" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A35,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Sheffield Ave &amp; Waveland Ave</v>
       </c>
       <c r="E35" t="str">
         <f>IF(AND(D35="same",C35="same"),"missing",IF(B35=D35,"same",IF(AND(A35&lt;&gt;C35,D35="same"),"id",IF(B35&lt;&gt;D35,"name"))))</f>
-        <v>missing</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>name</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>614</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="C36" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B36,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21690,19 +21459,19 @@
       </c>
       <c r="D36" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A36,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Ashland Ave &amp; Lake St</v>
       </c>
       <c r="E36" t="str">
         <f>IF(AND(D36="same",C36="same"),"missing",IF(B36=D36,"same",IF(AND(A36&lt;&gt;C36,D36="same"),"id",IF(B36&lt;&gt;D36,"name"))))</f>
-        <v>missing</v>
+        <v>name</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>574</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>39</v>
       </c>
       <c r="C37" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B37,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21710,7 +21479,7 @@
       </c>
       <c r="D37" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A37,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Vernon Ave &amp; 79th St</v>
+        <v>Wentworth Ave &amp; Cermak Rd</v>
       </c>
       <c r="E37" t="str">
         <f>IF(AND(D37="same",C37="same"),"missing",IF(B37=D37,"same",IF(AND(A37&lt;&gt;C37,D37="same"),"id",IF(B37&lt;&gt;D37,"name"))))</f>
@@ -21719,10 +21488,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>650</v>
+        <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="C38" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B38,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21730,7 +21499,7 @@
       </c>
       <c r="D38" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A38,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Eggleston Ave &amp; 69th St</v>
+        <v>Wentworth Ave &amp; Cermak Rd</v>
       </c>
       <c r="E38" t="str">
         <f>IF(AND(D38="same",C38="same"),"missing",IF(B38=D38,"same",IF(AND(A38&lt;&gt;C38,D38="same"),"id",IF(B38&lt;&gt;D38,"name"))))</f>
@@ -21739,10 +21508,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>635</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>137</v>
+        <v>41</v>
       </c>
       <c r="C39" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B39,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21750,7 +21519,7 @@
       </c>
       <c r="D39" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A39,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Fairbanks St &amp; Superior St</v>
+        <v>Wentworth Ave &amp; 24th St Temp</v>
       </c>
       <c r="E39" t="str">
         <f>IF(AND(D39="same",C39="same"),"missing",IF(B39=D39,"same",IF(AND(A39&lt;&gt;C39,D39="same"),"id",IF(B39&lt;&gt;D39,"name"))))</f>
@@ -21759,10 +21528,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>89</v>
+        <v>157</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C40" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B40,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21770,7 +21539,7 @@
       </c>
       <c r="D40" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A40,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Financial Pl &amp; Ida B Wells Dr</v>
+        <v>DuSable Lake Shore Dr &amp; Wellington Ave</v>
       </c>
       <c r="E40" t="str">
         <f>IF(AND(D40="same",C40="same"),"missing",IF(B40=D40,"same",IF(AND(A40&lt;&gt;C40,D40="same"),"id",IF(B40&lt;&gt;D40,"name"))))</f>
@@ -21779,10 +21548,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>89</v>
+        <v>179</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C41" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B41,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21790,7 +21559,7 @@
       </c>
       <c r="D41" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A41,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Financial Pl &amp; Ida B Wells Dr</v>
+        <v>MLK Jr Dr &amp; Pershing Rd</v>
       </c>
       <c r="E41" t="str">
         <f>IF(AND(D41="same",C41="same"),"missing",IF(B41=D41,"same",IF(AND(A41&lt;&gt;C41,D41="same"),"id",IF(B41&lt;&gt;D41,"name"))))</f>
@@ -21799,10 +21568,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>89</v>
+        <v>183</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C42" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B42,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21810,19 +21579,19 @@
       </c>
       <c r="D42" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A42,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Financial Pl &amp; Ida B Wells Dr</v>
+        <v>Damen Ave &amp; Thomas St Augusta Blvd</v>
       </c>
       <c r="E42" t="str">
         <f>IF(AND(D42="same",C42="same"),"missing",IF(B42=D42,"same",IF(AND(A42&lt;&gt;C42,D42="same"),"id",IF(B42&lt;&gt;D42,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>606</v>
+        <v>191</v>
       </c>
       <c r="B43" t="s">
-        <v>119</v>
+        <v>45</v>
       </c>
       <c r="C43" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B43,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21830,19 +21599,19 @@
       </c>
       <c r="D43" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A43,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Canal St &amp; Monroe St</v>
       </c>
       <c r="E43" t="str">
         <f>IF(AND(D43="same",C43="same"),"missing",IF(B43=D43,"same",IF(AND(A43&lt;&gt;C43,D43="same"),"id",IF(B43&lt;&gt;D43,"name"))))</f>
-        <v>missing</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>name</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>609</v>
+        <v>198</v>
       </c>
       <c r="B44" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="C44" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B44,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21850,19 +21619,19 @@
       </c>
       <c r="D44" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A44,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Green St &amp; Madison St</v>
       </c>
       <c r="E44" t="str">
         <f>IF(AND(D44="same",C44="same"),"missing",IF(B44=D44,"same",IF(AND(A44&lt;&gt;C44,D44="same"),"id",IF(B44&lt;&gt;D44,"name"))))</f>
-        <v>missing</v>
+        <v>name</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>287</v>
+        <v>198</v>
       </c>
       <c r="B45" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C45" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B45,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21870,7 +21639,7 @@
       </c>
       <c r="D45" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A45,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Franklin St &amp; Monroe St</v>
+        <v>Green St &amp; Madison St</v>
       </c>
       <c r="E45" t="str">
         <f>IF(AND(D45="same",C45="same"),"missing",IF(B45=D45,"same",IF(AND(A45&lt;&gt;C45,D45="same"),"id",IF(B45&lt;&gt;D45,"name"))))</f>
@@ -21879,10 +21648,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>31</v>
+        <v>208</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C46" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B46,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21890,7 +21659,7 @@
       </c>
       <c r="D46" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A46,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Franklin St &amp; Chicago Ave</v>
+        <v>Laflin St &amp; Cullerton St</v>
       </c>
       <c r="E46" t="str">
         <f>IF(AND(D46="same",C46="same"),"missing",IF(B46=D46,"same",IF(AND(A46&lt;&gt;C46,D46="same"),"id",IF(B46&lt;&gt;D46,"name"))))</f>
@@ -21899,10 +21668,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>286</v>
+        <v>211</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C47" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B47,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21910,7 +21679,7 @@
       </c>
       <c r="D47" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A47,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Franklin St &amp; Adams St Temp</v>
+        <v>St. Clair St &amp; Erie St</v>
       </c>
       <c r="E47" t="str">
         <f>IF(AND(D47="same",C47="same"),"missing",IF(B47=D47,"same",IF(AND(A47&lt;&gt;C47,D47="same"),"id",IF(B47&lt;&gt;D47,"name"))))</f>
@@ -21919,10 +21688,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C48" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B48,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21930,7 +21699,7 @@
       </c>
       <c r="D48" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A48,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Green St &amp; Madison St</v>
+        <v>Wells St &amp; Hubbard St</v>
       </c>
       <c r="E48" t="str">
         <f>IF(AND(D48="same",C48="same"),"missing",IF(B48=D48,"same",IF(AND(A48&lt;&gt;C48,D48="same"),"id",IF(B48&lt;&gt;D48,"name"))))</f>
@@ -21939,10 +21708,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>279</v>
+        <v>217</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C49" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B49,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21950,7 +21719,7 @@
       </c>
       <c r="D49" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A49,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Halsted St &amp; 35th St</v>
+        <v>Elizabeth May St &amp; Fulton St</v>
       </c>
       <c r="E49" t="str">
         <f>IF(AND(D49="same",C49="same"),"missing",IF(B49=D49,"same",IF(AND(A49&lt;&gt;C49,D49="same"),"id",IF(B49&lt;&gt;D49,"name"))))</f>
@@ -21959,10 +21728,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>331</v>
+        <v>217</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="C50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B50,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21970,7 +21739,7 @@
       </c>
       <c r="D50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A50,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Halsted St &amp; Clybourn Ave</v>
+        <v>Elizabeth May St &amp; Fulton St</v>
       </c>
       <c r="E50" t="str">
         <f>IF(AND(D50="same",C50="same"),"missing",IF(B50=D50,"same",IF(AND(A50&lt;&gt;C50,D50="same"),"id",IF(B50&lt;&gt;D50,"name"))))</f>
@@ -21979,10 +21748,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>331</v>
+        <v>220</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C51" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B51,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -21990,7 +21759,7 @@
       </c>
       <c r="D51" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A51,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Halsted St &amp; Clybourn Ave</v>
+        <v>Clark St &amp; Drummond Pl</v>
       </c>
       <c r="E51" t="str">
         <f>IF(AND(D51="same",C51="same"),"missing",IF(B51=D51,"same",IF(AND(A51&lt;&gt;C51,D51="same"),"id",IF(B51&lt;&gt;D51,"name"))))</f>
@@ -21999,10 +21768,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>331</v>
+        <v>233</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="C52" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B52,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22010,7 +21779,7 @@
       </c>
       <c r="D52" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A52,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Halsted St &amp; Clybourn Ave</v>
+        <v>Sangamon St &amp; Washington Blvd</v>
       </c>
       <c r="E52" t="str">
         <f>IF(AND(D52="same",C52="same"),"missing",IF(B52=D52,"same",IF(AND(A52&lt;&gt;C52,D52="same"),"id",IF(B52&lt;&gt;D52,"name"))))</f>
@@ -22019,10 +21788,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>332</v>
+        <v>238</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="C53" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B53,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22030,7 +21799,7 @@
       </c>
       <c r="D53" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A53,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Burling St &amp; Diversey Pkwy</v>
+        <v>Wolcott Ravenswood Ave &amp; Montrose Ave</v>
       </c>
       <c r="E53" t="str">
         <f>IF(AND(D53="same",C53="same"),"missing",IF(B53=D53,"same",IF(AND(A53&lt;&gt;C53,D53="same"),"id",IF(B53&lt;&gt;D53,"name"))))</f>
@@ -22039,10 +21808,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>55</v>
+        <v>238</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C54" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B54,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22050,7 +21819,7 @@
       </c>
       <c r="D54" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A54,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Halsted St &amp; Roosevelt Rd</v>
+        <v>Wolcott Ravenswood Ave &amp; Montrose Ave</v>
       </c>
       <c r="E54" t="str">
         <f>IF(AND(D54="same",C54="same"),"missing",IF(B54=D54,"same",IF(AND(A54&lt;&gt;C54,D54="same"),"id",IF(B54&lt;&gt;D54,"name"))))</f>
@@ -22059,10 +21828,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C55" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B55,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22070,7 +21839,7 @@
       </c>
       <c r="D55" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A55,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Green St &amp; Madison St</v>
+        <v>Wolcott Ravenswood Ave &amp; Montrose Ave</v>
       </c>
       <c r="E55" t="str">
         <f>IF(AND(D55="same",C55="same"),"missing",IF(B55=D55,"same",IF(AND(A55&lt;&gt;C55,D55="same"),"id",IF(B55&lt;&gt;D55,"name"))))</f>
@@ -22079,10 +21848,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>304</v>
+        <v>243</v>
       </c>
       <c r="B56" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C56" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B56,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22090,7 +21859,7 @@
       </c>
       <c r="D56" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A56,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Broadway &amp; Waveland Ave</v>
+        <v>Lincoln Ave &amp; Sunnyside Ave</v>
       </c>
       <c r="E56" t="str">
         <f>IF(AND(D56="same",C56="same"),"missing",IF(B56=D56,"same",IF(AND(A56&lt;&gt;C56,D56="same"),"id",IF(B56&lt;&gt;D56,"name"))))</f>
@@ -22099,10 +21868,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>220</v>
+        <v>247</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C57" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B57,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22110,19 +21879,19 @@
       </c>
       <c r="D57" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A57,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Clark St &amp; Drummond Pl</v>
+        <v>Shore Dr &amp; 55th St</v>
       </c>
       <c r="E57" t="str">
         <f>IF(AND(D57="same",C57="same"),"missing",IF(B57=D57,"same",IF(AND(A57&lt;&gt;C57,D57="same"),"id",IF(B57&lt;&gt;D57,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>671</v>
+        <v>253</v>
       </c>
       <c r="B58" t="s">
-        <v>152</v>
+        <v>60</v>
       </c>
       <c r="C58" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B58,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22130,19 +21899,19 @@
       </c>
       <c r="D58" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A58,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Winthrop Ave &amp; Lawrence Ave</v>
       </c>
       <c r="E58" t="str">
         <f>IF(AND(D58="same",C58="same"),"missing",IF(B58=D58,"same",IF(AND(A58&lt;&gt;C58,D58="same"),"id",IF(B58&lt;&gt;D58,"name"))))</f>
-        <v>missing</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>name</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>372</v>
+        <v>259</v>
       </c>
       <c r="B59" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="C59" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B59,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22150,19 +21919,19 @@
       </c>
       <c r="D59" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A59,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>California Ave &amp; Francis Pl Temp</v>
       </c>
       <c r="E59" t="str">
         <f>IF(AND(D59="same",C59="same"),"missing",IF(B59=D59,"same",IF(AND(A59&lt;&gt;C59,D59="same"),"id",IF(B59&lt;&gt;D59,"name"))))</f>
-        <v>missing</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>name</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>608</v>
+        <v>268</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
       <c r="C60" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B60,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22170,19 +21939,19 @@
       </c>
       <c r="D60" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A60,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>DuSable Lake Shore Dr &amp; North Blvd</v>
       </c>
       <c r="E60" t="str">
         <f>IF(AND(D60="same",C60="same"),"missing",IF(B60=D60,"same",IF(AND(A60&lt;&gt;C60,D60="same"),"id",IF(B60&lt;&gt;D60,"name"))))</f>
-        <v>missing</v>
+        <v>name</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>480</v>
+        <v>273</v>
       </c>
       <c r="B61" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="C61" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B61,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22190,7 +21959,7 @@
       </c>
       <c r="D61" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A61,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Albany Ave &amp; Montrose Ave</v>
+        <v>Michigan Ave &amp; 18th St</v>
       </c>
       <c r="E61" t="str">
         <f>IF(AND(D61="same",C61="same"),"missing",IF(B61=D61,"same",IF(AND(A61&lt;&gt;C61,D61="same"),"id",IF(B61&lt;&gt;D61,"name"))))</f>
@@ -22199,10 +21968,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>483</v>
+        <v>278</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="C62" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B62,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22210,7 +21979,7 @@
       </c>
       <c r="D62" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A62,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Avondale Ave &amp; Irving Park Rd</v>
+        <v>Wallace St &amp; 35th St</v>
       </c>
       <c r="E62" t="str">
         <f>IF(AND(D62="same",C62="same"),"missing",IF(B62=D62,"same",IF(AND(A62&lt;&gt;C62,D62="same"),"id",IF(B62&lt;&gt;D62,"name"))))</f>
@@ -22219,10 +21988,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>334</v>
+        <v>279</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C63" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B63,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22230,7 +21999,7 @@
       </c>
       <c r="D63" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A63,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>DuSable Lake Shore Dr &amp; Belmont Ave</v>
+        <v>Halsted St &amp; 35th St</v>
       </c>
       <c r="E63" t="str">
         <f>IF(AND(D63="same",C63="same"),"missing",IF(B63=D63,"same",IF(AND(A63&lt;&gt;C63,D63="same"),"id",IF(B63&lt;&gt;D63,"name"))))</f>
@@ -22239,10 +22008,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>329</v>
+        <v>285</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C64" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B64,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22250,7 +22019,7 @@
       </c>
       <c r="D64" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A64,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>DuSable Lake Shore Dr &amp; Diversey Pkwy</v>
+        <v>Wood St &amp; Hubbard St</v>
       </c>
       <c r="E64" t="str">
         <f>IF(AND(D64="same",C64="same"),"missing",IF(B64=D64,"same",IF(AND(A64&lt;&gt;C64,D64="same"),"id",IF(B64&lt;&gt;D64,"name"))))</f>
@@ -22259,10 +22028,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>76</v>
+        <v>286</v>
       </c>
       <c r="B65" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C65" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B65,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22270,7 +22039,7 @@
       </c>
       <c r="D65" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A65,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>DuSable Lake Shore Dr &amp; Monroe St</v>
+        <v>Franklin St &amp; Adams St Temp</v>
       </c>
       <c r="E65" t="str">
         <f>IF(AND(D65="same",C65="same"),"missing",IF(B65=D65,"same",IF(AND(A65&lt;&gt;C65,D65="same"),"id",IF(B65&lt;&gt;D65,"name"))))</f>
@@ -22279,10 +22048,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="B66" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C66" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B66,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22290,7 +22059,7 @@
       </c>
       <c r="D66" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A66,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>DuSable Lake Shore Dr &amp; North Blvd</v>
+        <v>Franklin St &amp; Monroe St</v>
       </c>
       <c r="E66" t="str">
         <f>IF(AND(D66="same",C66="same"),"missing",IF(B66=D66,"same",IF(AND(A66&lt;&gt;C66,D66="same"),"id",IF(B66&lt;&gt;D66,"name"))))</f>
@@ -22299,10 +22068,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>99</v>
+        <v>289</v>
       </c>
       <c r="B67" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="C67" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B67,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22310,7 +22079,7 @@
       </c>
       <c r="D67" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A67,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>McClurg Ct &amp; Ohio St</v>
+        <v>Wells St &amp; Concord Ln</v>
       </c>
       <c r="E67" t="str">
         <f>IF(AND(D67="same",C67="same"),"missing",IF(B67=D67,"same",IF(AND(A67&lt;&gt;C67,D67="same"),"id",IF(B67&lt;&gt;D67,"name"))))</f>
@@ -22319,10 +22088,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>157</v>
+        <v>293</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="C68" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B68,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22330,39 +22099,39 @@
       </c>
       <c r="D68" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A68,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>DuSable Lake Shore Dr &amp; Wellington Ave</v>
+        <v>Broadway &amp; Wilson - Truman College Vaccination Site</v>
       </c>
       <c r="E68" t="str">
         <f>IF(AND(D68="same",C68="same"),"missing",IF(B68=D68,"same",IF(AND(A68&lt;&gt;C68,D68="same"),"id",IF(B68&lt;&gt;D68,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>459</v>
+        <v>304</v>
       </c>
       <c r="B69" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="C69" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B69,0),Stations!$B:$D,2,FALSE),"same")</f>
-        <v>760</v>
+        <v>same</v>
       </c>
       <c r="D69" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A69,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Broadway &amp; Waveland Ave</v>
       </c>
       <c r="E69" t="str">
         <f>IF(AND(D69="same",C69="same"),"missing",IF(B69=D69,"same",IF(AND(A69&lt;&gt;C69,D69="same"),"id",IF(B69&lt;&gt;D69,"name"))))</f>
-        <v>id</v>
+        <v>name</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>53</v>
+        <v>315</v>
       </c>
       <c r="B70" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="C70" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B70,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22370,7 +22139,7 @@
       </c>
       <c r="D70" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A70,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wells St &amp; Huron St</v>
+        <v>Elston Ave &amp; Wabansia Ave</v>
       </c>
       <c r="E70" t="str">
         <f>IF(AND(D70="same",C70="same"),"missing",IF(B70=D70,"same",IF(AND(A70&lt;&gt;C70,D70="same"),"id",IF(B70&lt;&gt;D70,"name"))))</f>
@@ -22379,10 +22148,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>627</v>
+        <v>317</v>
       </c>
       <c r="B71" t="s">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="C71" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B71,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22390,7 +22159,7 @@
       </c>
       <c r="D71" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A71,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>LaSalle Dr &amp; Huron St</v>
+        <v>Wood St &amp; Taylor St Temp</v>
       </c>
       <c r="E71" t="str">
         <f>IF(AND(D71="same",C71="same"),"missing",IF(B71=D71,"same",IF(AND(A71&lt;&gt;C71,D71="same"),"id",IF(B71&lt;&gt;D71,"name"))))</f>
@@ -22399,10 +22168,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>440</v>
+        <v>321</v>
       </c>
       <c r="B72" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C72" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B72,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22410,19 +22179,19 @@
       </c>
       <c r="D72" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A72,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Central Park Ave &amp; 24th St</v>
+        <v>Wabash Ave &amp; 9th St</v>
       </c>
       <c r="E72" t="str">
         <f>IF(AND(D72="same",C72="same"),"missing",IF(B72=D72,"same",IF(AND(A72&lt;&gt;C72,D72="same"),"id",IF(B72&lt;&gt;D72,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>669</v>
+        <v>325</v>
       </c>
       <c r="B73" t="s">
-        <v>151</v>
+        <v>75</v>
       </c>
       <c r="C73" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B73,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22430,19 +22199,19 @@
       </c>
       <c r="D73" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A73,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Clark St &amp; Winnemac Ave</v>
       </c>
       <c r="E73" t="str">
         <f>IF(AND(D73="same",C73="same"),"missing",IF(B73=D73,"same",IF(AND(A73&lt;&gt;C73,D73="same"),"id",IF(B73&lt;&gt;D73,"name"))))</f>
-        <v>missing</v>
+        <v>name</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>664</v>
+        <v>329</v>
       </c>
       <c r="B74" t="s">
-        <v>150</v>
+        <v>76</v>
       </c>
       <c r="C74" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B74,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22450,7 +22219,7 @@
       </c>
       <c r="D74" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A74,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Leavitt St &amp; Belmont Ave</v>
+        <v>DuSable Lake Shore Dr &amp; Diversey Pkwy</v>
       </c>
       <c r="E74" t="str">
         <f>IF(AND(D74="same",C74="same"),"missing",IF(B74=D74,"same",IF(AND(A74&lt;&gt;C74,D74="same"),"id",IF(B74&lt;&gt;D74,"name"))))</f>
@@ -22459,10 +22228,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>658</v>
+        <v>331</v>
       </c>
       <c r="B75" t="s">
-        <v>149</v>
+        <v>77</v>
       </c>
       <c r="C75" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B75,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22470,7 +22239,7 @@
       </c>
       <c r="D75" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A75,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Leavitt St &amp; Division St</v>
+        <v>Halsted St &amp; Clybourn Ave</v>
       </c>
       <c r="E75" t="str">
         <f>IF(AND(D75="same",C75="same"),"missing",IF(B75=D75,"same",IF(AND(A75&lt;&gt;C75,D75="same"),"id",IF(B75&lt;&gt;D75,"name"))))</f>
@@ -22479,10 +22248,10 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>315</v>
+        <v>331</v>
       </c>
       <c r="B76" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C76" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B76,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22490,7 +22259,7 @@
       </c>
       <c r="D76" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A76,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Elston Ave &amp; Wabansia Ave</v>
+        <v>Halsted St &amp; Clybourn Ave</v>
       </c>
       <c r="E76" t="str">
         <f>IF(AND(D76="same",C76="same"),"missing",IF(B76=D76,"same",IF(AND(A76&lt;&gt;C76,D76="same"),"id",IF(B76&lt;&gt;D76,"name"))))</f>
@@ -22499,10 +22268,10 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>243</v>
+        <v>331</v>
       </c>
       <c r="B77" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="C77" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B77,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22510,19 +22279,19 @@
       </c>
       <c r="D77" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A77,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Lincoln Ave &amp; Sunnyside Ave</v>
+        <v>Halsted St &amp; Clybourn Ave</v>
       </c>
       <c r="E77" t="str">
         <f>IF(AND(D77="same",C77="same"),"missing",IF(B77=D77,"same",IF(AND(A77&lt;&gt;C77,D77="same"),"id",IF(B77&lt;&gt;D77,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>618</v>
+        <v>332</v>
       </c>
       <c r="B78" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="C78" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B78,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22530,19 +22299,19 @@
       </c>
       <c r="D78" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A78,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Burling St &amp; Diversey Pkwy</v>
       </c>
       <c r="E78" t="str">
         <f>IF(AND(D78="same",C78="same"),"missing",IF(B78=D78,"same",IF(AND(A78&lt;&gt;C78,D78="same"),"id",IF(B78&lt;&gt;D78,"name"))))</f>
-        <v>missing</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>name</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>615</v>
+        <v>332</v>
       </c>
       <c r="B79" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="C79" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B79,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22550,19 +22319,19 @@
       </c>
       <c r="D79" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A79,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Burling St &amp; Diversey Pkwy</v>
       </c>
       <c r="E79" t="str">
         <f>IF(AND(D79="same",C79="same"),"missing",IF(B79=D79,"same",IF(AND(A79&lt;&gt;C79,D79="same"),"id",IF(B79&lt;&gt;D79,"name"))))</f>
-        <v>missing</v>
+        <v>name</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>19</v>
+        <v>334</v>
       </c>
       <c r="B80" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="C80" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B80,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22570,7 +22339,7 @@
       </c>
       <c r="D80" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A80,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Throop St &amp; Taylor St</v>
+        <v>DuSable Lake Shore Dr &amp; Belmont Ave</v>
       </c>
       <c r="E80" t="str">
         <f>IF(AND(D80="same",C80="same"),"missing",IF(B80=D80,"same",IF(AND(A80&lt;&gt;C80,D80="same"),"id",IF(B80&lt;&gt;D80,"name"))))</f>
@@ -22579,10 +22348,10 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>19</v>
+        <v>360</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="C81" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B81,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22590,19 +22359,19 @@
       </c>
       <c r="D81" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A81,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Throop St &amp; Taylor St</v>
+        <v>same</v>
       </c>
       <c r="E81" t="str">
         <f>IF(AND(D81="same",C81="same"),"missing",IF(B81=D81,"same",IF(AND(A81&lt;&gt;C81,D81="same"),"id",IF(B81&lt;&gt;D81,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>631</v>
+        <v>361</v>
       </c>
       <c r="B82" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="C82" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B82,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22610,19 +22379,19 @@
       </c>
       <c r="D82" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A82,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Malcolm X College Vaccination Site</v>
+        <v>same</v>
       </c>
       <c r="E82" t="str">
         <f>IF(AND(D82="same",C82="same"),"missing",IF(B82=D82,"same",IF(AND(A82&lt;&gt;C82,D82="same"),"id",IF(B82&lt;&gt;D82,"name"))))</f>
-        <v>name</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>missing</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>610</v>
+        <v>363</v>
       </c>
       <c r="B83" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="C83" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B83,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22639,10 +22408,10 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>58</v>
+        <v>372</v>
       </c>
       <c r="B84" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="C84" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B84,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22650,19 +22419,19 @@
       </c>
       <c r="D84" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A84,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Elston Ave &amp; Cortland St</v>
+        <v>same</v>
       </c>
       <c r="E84" t="str">
         <f>IF(AND(D84="same",C84="same"),"missing",IF(B84=D84,"same",IF(AND(A84&lt;&gt;C84,D84="same"),"id",IF(B84&lt;&gt;D84,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>544</v>
+        <v>372</v>
       </c>
       <c r="B85" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="C85" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B85,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22670,19 +22439,19 @@
       </c>
       <c r="D85" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A85,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Austin Blvd &amp; Madison St</v>
+        <v>same</v>
       </c>
       <c r="E85" t="str">
         <f>IF(AND(D85="same",C85="same"),"missing",IF(B85=D85,"same",IF(AND(A85&lt;&gt;C85,D85="same"),"id",IF(B85&lt;&gt;D85,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>217</v>
+        <v>383</v>
       </c>
       <c r="B86" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="C86" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B86,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22690,7 +22459,7 @@
       </c>
       <c r="D86" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A86,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Elizabeth May St &amp; Fulton St</v>
+        <v>Paulina St &amp; Flournoy St</v>
       </c>
       <c r="E86" t="str">
         <f>IF(AND(D86="same",C86="same"),"missing",IF(B86=D86,"same",IF(AND(A86&lt;&gt;C86,D86="same"),"id",IF(B86&lt;&gt;D86,"name"))))</f>
@@ -22699,10 +22468,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>88</v>
+        <v>397</v>
       </c>
       <c r="B87" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="C87" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B87,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22710,19 +22479,19 @@
       </c>
       <c r="D87" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A87,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Racine Ave &amp; Randolph St</v>
+        <v>same</v>
       </c>
       <c r="E87" t="str">
         <f>IF(AND(D87="same",C87="same"),"missing",IF(B87=D87,"same",IF(AND(A87&lt;&gt;C87,D87="same"),"id",IF(B87&lt;&gt;D87,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>26</v>
+        <v>402</v>
       </c>
       <c r="B88" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="C88" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B88,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22730,7 +22499,7 @@
       </c>
       <c r="D88" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A88,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>New St &amp; Illinois St</v>
+        <v>Shields Ave &amp; 31st St</v>
       </c>
       <c r="E88" t="str">
         <f>IF(AND(D88="same",C88="same"),"missing",IF(B88=D88,"same",IF(AND(A88&lt;&gt;C88,D88="same"),"id",IF(B88&lt;&gt;D88,"name"))))</f>
@@ -22739,10 +22508,10 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>273</v>
+        <v>408</v>
       </c>
       <c r="B89" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C89" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B89,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22750,39 +22519,39 @@
       </c>
       <c r="D89" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A89,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Michigan Ave &amp; 18th St</v>
+        <v>Union Ave &amp; Root St</v>
       </c>
       <c r="E89" t="str">
         <f>IF(AND(D89="same",C89="same"),"missing",IF(B89=D89,"same",IF(AND(A89&lt;&gt;C89,D89="same"),"id",IF(B89&lt;&gt;D89,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>651</v>
+        <v>414</v>
       </c>
       <c r="B90" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="C90" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B90,0),Stations!$B:$D,2,FALSE),"same")</f>
-        <v>674</v>
+        <v>same</v>
       </c>
       <c r="D90" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A90,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Canal St &amp; Taylor St</v>
       </c>
       <c r="E90" t="str">
         <f>IF(AND(D90="same",C90="same"),"missing",IF(B90=D90,"same",IF(AND(A90&lt;&gt;C90,D90="same"),"id",IF(B90&lt;&gt;D90,"name"))))</f>
-        <v>id</v>
+        <v>name</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>2</v>
+        <v>417</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C91" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B91,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22790,7 +22559,7 @@
       </c>
       <c r="D91" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A91,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Buckingham Fountain</v>
+        <v>Cornell Ave &amp; Hyde Park Blvd</v>
       </c>
       <c r="E91" t="str">
         <f>IF(AND(D91="same",C91="same"),"missing",IF(B91=D91,"same",IF(AND(A91&lt;&gt;C91,D91="same"),"id",IF(B91&lt;&gt;D91,"name"))))</f>
@@ -22799,10 +22568,10 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>45</v>
+        <v>421</v>
       </c>
       <c r="B92" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="C92" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B92,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22810,7 +22579,7 @@
       </c>
       <c r="D92" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A92,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Michigan Ave &amp; Ida B Wells Dr</v>
+        <v>MLK Jr Dr &amp; 56th St</v>
       </c>
       <c r="E92" t="str">
         <f>IF(AND(D92="same",C92="same"),"missing",IF(B92=D92,"same",IF(AND(A92&lt;&gt;C92,D92="same"),"id",IF(B92&lt;&gt;D92,"name"))))</f>
@@ -22819,10 +22588,10 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>421</v>
+        <v>436</v>
       </c>
       <c r="B93" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C93" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B93,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22830,7 +22599,7 @@
       </c>
       <c r="D93" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A93,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>MLK Jr Dr &amp; 56th St</v>
+        <v>Fairfield Ave &amp; Roosevelt Rd</v>
       </c>
       <c r="E93" t="str">
         <f>IF(AND(D93="same",C93="same"),"missing",IF(B93=D93,"same",IF(AND(A93&lt;&gt;C93,D93="same"),"id",IF(B93&lt;&gt;D93,"name"))))</f>
@@ -22839,10 +22608,10 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>179</v>
+        <v>437</v>
       </c>
       <c r="B94" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="C94" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B94,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22850,7 +22619,7 @@
       </c>
       <c r="D94" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A94,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>MLK Jr Dr &amp; Pershing Rd</v>
+        <v>Washtenaw Ave &amp; Ogden Ave</v>
       </c>
       <c r="E94" t="str">
         <f>IF(AND(D94="same",C94="same"),"missing",IF(B94=D94,"same",IF(AND(A94&lt;&gt;C94,D94="same"),"id",IF(B94&lt;&gt;D94,"name"))))</f>
@@ -22859,10 +22628,10 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
+        <v>437</v>
+      </c>
+      <c r="B95" t="s">
         <v>97</v>
-      </c>
-      <c r="B95" t="s">
-        <v>32</v>
       </c>
       <c r="C95" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B95,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22870,19 +22639,19 @@
       </c>
       <c r="D95" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A95,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Field Museum</v>
+        <v>Washtenaw Ave &amp; Ogden Ave</v>
       </c>
       <c r="E95" t="str">
         <f>IF(AND(D95="same",C95="same"),"missing",IF(B95=D95,"same",IF(AND(A95&lt;&gt;C95,D95="same"),"id",IF(B95&lt;&gt;D95,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>616</v>
+        <v>437</v>
       </c>
       <c r="B96" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="C96" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B96,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22890,19 +22659,19 @@
       </c>
       <c r="D96" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A96,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Washtenaw Ave &amp; Ogden Ave</v>
       </c>
       <c r="E96" t="str">
         <f>IF(AND(D96="same",C96="same"),"missing",IF(B96=D96,"same",IF(AND(A96&lt;&gt;C96,D96="same"),"id",IF(B96&lt;&gt;D96,"name"))))</f>
-        <v>missing</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>name</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>611</v>
+        <v>440</v>
       </c>
       <c r="B97" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C97" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B97,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22910,19 +22679,19 @@
       </c>
       <c r="D97" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A97,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Central Park Ave &amp; 24th St</v>
       </c>
       <c r="E97" t="str">
         <f>IF(AND(D97="same",C97="same"),"missing",IF(B97=D97,"same",IF(AND(A97&lt;&gt;C97,D97="same"),"id",IF(B97&lt;&gt;D97,"name"))))</f>
-        <v>missing</v>
+        <v>name</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>493</v>
+        <v>446</v>
       </c>
       <c r="B98" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C98" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B98,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22930,7 +22699,7 @@
       </c>
       <c r="D98" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A98,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Western Ave &amp; Roscoe St</v>
+        <v>Western &amp; 28th - Velasquez Institute Vaccination Site</v>
       </c>
       <c r="E98" t="str">
         <f>IF(AND(D98="same",C98="same"),"missing",IF(B98=D98,"same",IF(AND(A98&lt;&gt;C98,D98="same"),"id",IF(B98&lt;&gt;D98,"name"))))</f>
@@ -22939,30 +22708,30 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>23</v>
+        <v>459</v>
       </c>
       <c r="B99" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="C99" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B99,0),Stations!$B:$D,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>760</v>
       </c>
       <c r="D99" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A99,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Orleans St &amp; Elm St</v>
+        <v>same</v>
       </c>
       <c r="E99" t="str">
         <f>IF(AND(D99="same",C99="same"),"missing",IF(B99=D99,"same",IF(AND(A99&lt;&gt;C99,D99="same"),"id",IF(B99&lt;&gt;D99,"name"))))</f>
-        <v>name</v>
+        <v>id</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>636</v>
+        <v>462</v>
       </c>
       <c r="B100" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="C100" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B100,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22970,7 +22739,7 @@
       </c>
       <c r="D100" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A100,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Orleans St &amp; Hubbard St</v>
+        <v>Winchester Ravenswood Ave &amp; Balmoral Ave</v>
       </c>
       <c r="E100" t="str">
         <f>IF(AND(D100="same",C100="same"),"missing",IF(B100=D100,"same",IF(AND(A100&lt;&gt;C100,D100="same"),"id",IF(B100&lt;&gt;D100,"name"))))</f>
@@ -22979,10 +22748,10 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>212</v>
+        <v>480</v>
       </c>
       <c r="B101" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="C101" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B101,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -22990,7 +22759,7 @@
       </c>
       <c r="D101" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A101,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wells St &amp; Hubbard St</v>
+        <v>Albany Ave &amp; Montrose Ave</v>
       </c>
       <c r="E101" t="str">
         <f>IF(AND(D101="same",C101="same"),"missing",IF(B101=D101,"same",IF(AND(A101&lt;&gt;C101,D101="same"),"id",IF(B101&lt;&gt;D101,"name"))))</f>
@@ -22999,10 +22768,10 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>16</v>
+        <v>480</v>
       </c>
       <c r="B102" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="C102" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B102,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23010,7 +22779,7 @@
       </c>
       <c r="D102" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A102,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Paulina Ave &amp; North Ave</v>
+        <v>Albany Ave &amp; Montrose Ave</v>
       </c>
       <c r="E102" t="str">
         <f>IF(AND(D102="same",C102="same"),"missing",IF(B102=D102,"same",IF(AND(A102&lt;&gt;C102,D102="same"),"id",IF(B102&lt;&gt;D102,"name"))))</f>
@@ -23019,10 +22788,10 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>582</v>
+        <v>483</v>
       </c>
       <c r="B103" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C103" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B103,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23030,7 +22799,7 @@
       </c>
       <c r="D103" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A103,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Phillips Ave &amp; 83rd St</v>
+        <v>Avondale Ave &amp; Irving Park Rd</v>
       </c>
       <c r="E103" t="str">
         <f>IF(AND(D103="same",C103="same"),"missing",IF(B103=D103,"same",IF(AND(A103&lt;&gt;C103,D103="same"),"id",IF(B103&lt;&gt;D103,"name"))))</f>
@@ -23039,10 +22808,10 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>402</v>
+        <v>488</v>
       </c>
       <c r="B104" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="C104" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B104,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23050,7 +22819,7 @@
       </c>
       <c r="D104" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A104,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Shields Ave &amp; 31st St</v>
+        <v>Pulaski Rd &amp; Eddy St Temp</v>
       </c>
       <c r="E104" t="str">
         <f>IF(AND(D104="same",C104="same"),"missing",IF(B104=D104,"same",IF(AND(A104&lt;&gt;C104,D104="same"),"id",IF(B104&lt;&gt;D104,"name"))))</f>
@@ -23059,10 +22828,10 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>414</v>
+        <v>488</v>
       </c>
       <c r="B105" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C105" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B105,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23070,7 +22839,7 @@
       </c>
       <c r="D105" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A105,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Canal St &amp; Taylor St</v>
+        <v>Pulaski Rd &amp; Eddy St Temp</v>
       </c>
       <c r="E105" t="str">
         <f>IF(AND(D105="same",C105="same"),"missing",IF(B105=D105,"same",IF(AND(A105&lt;&gt;C105,D105="same"),"id",IF(B105&lt;&gt;D105,"name"))))</f>
@@ -23079,10 +22848,10 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="B106" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C106" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B106,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23090,7 +22859,7 @@
       </c>
       <c r="D106" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A106,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Pulaski Rd &amp; Eddy St Temp</v>
+        <v>Western Ave &amp; Roscoe St</v>
       </c>
       <c r="E106" t="str">
         <f>IF(AND(D106="same",C106="same"),"missing",IF(B106=D106,"same",IF(AND(A106&lt;&gt;C106,D106="same"),"id",IF(B106&lt;&gt;D106,"name"))))</f>
@@ -23099,10 +22868,10 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>488</v>
+        <v>503</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C107" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B107,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23110,7 +22879,7 @@
       </c>
       <c r="D107" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A107,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Pulaski Rd &amp; Eddy St Temp</v>
+        <v>St. Louis Ave &amp; Fullerton Ave</v>
       </c>
       <c r="E107" t="str">
         <f>IF(AND(D107="same",C107="same"),"missing",IF(B107=D107,"same",IF(AND(A107&lt;&gt;C107,D107="same"),"id",IF(B107&lt;&gt;D107,"name"))))</f>
@@ -23119,10 +22888,10 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>534</v>
+        <v>512</v>
       </c>
       <c r="B108" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C108" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B108,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23130,19 +22899,19 @@
       </c>
       <c r="D108" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A108,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Karlov Ave &amp; Madison St</v>
+        <v>same</v>
       </c>
       <c r="E108" t="str">
         <f>IF(AND(D108="same",C108="same"),"missing",IF(B108=D108,"same",IF(AND(A108&lt;&gt;C108,D108="same"),"id",IF(B108&lt;&gt;D108,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>654</v>
+        <v>534</v>
       </c>
       <c r="B109" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="C109" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B109,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23150,7 +22919,7 @@
       </c>
       <c r="D109" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A109,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Racine Ave &amp; Washington Blvd</v>
+        <v>Karlov Ave &amp; Madison St</v>
       </c>
       <c r="E109" t="str">
         <f>IF(AND(D109="same",C109="same"),"missing",IF(B109=D109,"same",IF(AND(A109&lt;&gt;C109,D109="same"),"id",IF(B109&lt;&gt;D109,"name"))))</f>
@@ -23159,10 +22928,10 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>217</v>
+        <v>544</v>
       </c>
       <c r="B110" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="C110" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B110,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23170,7 +22939,7 @@
       </c>
       <c r="D110" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A110,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Elizabeth May St &amp; Fulton St</v>
+        <v>Austin Blvd &amp; Madison St</v>
       </c>
       <c r="E110" t="str">
         <f>IF(AND(D110="same",C110="same"),"missing",IF(B110=D110,"same",IF(AND(A110&lt;&gt;C110,D110="same"),"id",IF(B110&lt;&gt;D110,"name"))))</f>
@@ -23179,10 +22948,10 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>462</v>
+        <v>557</v>
       </c>
       <c r="B111" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="C111" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B111,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23190,7 +22959,7 @@
       </c>
       <c r="D111" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A111,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Winchester Ravenswood Ave &amp; Balmoral Ave</v>
+        <v>Seeley Ave &amp; Garfield Blvd</v>
       </c>
       <c r="E111" t="str">
         <f>IF(AND(D111="same",C111="same"),"missing",IF(B111=D111,"same",IF(AND(A111&lt;&gt;C111,D111="same"),"id",IF(B111&lt;&gt;D111,"name"))))</f>
@@ -23199,10 +22968,10 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>238</v>
+        <v>561</v>
       </c>
       <c r="B112" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="C112" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B112,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23210,7 +22979,7 @@
       </c>
       <c r="D112" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A112,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wolcott Ravenswood Ave &amp; Montrose Ave</v>
+        <v>Damen Ave &amp; 59th St</v>
       </c>
       <c r="E112" t="str">
         <f>IF(AND(D112="same",C112="same"),"missing",IF(B112=D112,"same",IF(AND(A112&lt;&gt;C112,D112="same"),"id",IF(B112&lt;&gt;D112,"name"))))</f>
@@ -23219,10 +22988,10 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>238</v>
+        <v>566</v>
       </c>
       <c r="B113" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="C113" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B113,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23230,19 +22999,19 @@
       </c>
       <c r="D113" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A113,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wolcott Ravenswood Ave &amp; Montrose Ave</v>
+        <v>Damen Ave &amp; 74th St</v>
       </c>
       <c r="E113" t="str">
         <f>IF(AND(D113="same",C113="same"),"missing",IF(B113=D113,"same",IF(AND(A113&lt;&gt;C113,D113="same"),"id",IF(B113&lt;&gt;D113,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>612</v>
+        <v>574</v>
       </c>
       <c r="B114" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C114" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B114,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23250,19 +23019,19 @@
       </c>
       <c r="D114" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A114,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Vernon Ave &amp; 79th St</v>
       </c>
       <c r="E114" t="str">
         <f>IF(AND(D114="same",C114="same"),"missing",IF(B114=D114,"same",IF(AND(A114&lt;&gt;C114,D114="same"),"id",IF(B114&lt;&gt;D114,"name"))))</f>
-        <v>missing</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>name</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>397</v>
+        <v>578</v>
       </c>
       <c r="B115" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C115" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B115,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23270,19 +23039,19 @@
       </c>
       <c r="D115" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A115,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Bennett Ave &amp; 79th St</v>
       </c>
       <c r="E115" t="str">
         <f>IF(AND(D115="same",C115="same"),"missing",IF(B115=D115,"same",IF(AND(A115&lt;&gt;C115,D115="same"),"id",IF(B115&lt;&gt;D115,"name"))))</f>
-        <v>missing</v>
+        <v>name</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>233</v>
+        <v>582</v>
       </c>
       <c r="B116" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="C116" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B116,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23290,7 +23059,7 @@
       </c>
       <c r="D116" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A116,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Sangamon St &amp; Washington Blvd</v>
+        <v>Phillips Ave &amp; 83rd St</v>
       </c>
       <c r="E116" t="str">
         <f>IF(AND(D116="same",C116="same"),"missing",IF(B116=D116,"same",IF(AND(A116&lt;&gt;C116,D116="same"),"id",IF(B116&lt;&gt;D116,"name"))))</f>
@@ -23299,10 +23068,10 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>114</v>
+        <v>606</v>
       </c>
       <c r="B117" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C117" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B117,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23310,19 +23079,19 @@
       </c>
       <c r="D117" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A117,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Sheffield Ave &amp; Waveland Ave</v>
+        <v>same</v>
       </c>
       <c r="E117" t="str">
         <f>IF(AND(D117="same",C117="same"),"missing",IF(B117=D117,"same",IF(AND(A117&lt;&gt;C117,D117="same"),"id",IF(B117&lt;&gt;D117,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>247</v>
+        <v>607</v>
       </c>
       <c r="B118" t="s">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="C118" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B118,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23330,19 +23099,19 @@
       </c>
       <c r="D118" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A118,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Shore Dr &amp; 55th St</v>
+        <v>same</v>
       </c>
       <c r="E118" t="str">
         <f>IF(AND(D118="same",C118="same"),"missing",IF(B118=D118,"same",IF(AND(A118&lt;&gt;C118,D118="same"),"id",IF(B118&lt;&gt;D118,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>643</v>
+        <v>608</v>
       </c>
       <c r="B119" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="C119" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B119,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23350,19 +23119,19 @@
       </c>
       <c r="D119" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A119,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Smith Park</v>
+        <v>same</v>
       </c>
       <c r="E119" t="str">
         <f>IF(AND(D119="same",C119="same"),"missing",IF(B119=D119,"same",IF(AND(A119&lt;&gt;C119,D119="same"),"id",IF(B119&lt;&gt;D119,"name"))))</f>
-        <v>name</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>missing</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>1</v>
+        <v>609</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="C120" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B120,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23379,10 +23148,10 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>211</v>
+        <v>610</v>
       </c>
       <c r="B121" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="C121" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B121,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23390,19 +23159,19 @@
       </c>
       <c r="D121" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A121,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>St. Clair St &amp; Erie St</v>
+        <v>same</v>
       </c>
       <c r="E121" t="str">
         <f>IF(AND(D121="same",C121="same"),"missing",IF(B121=D121,"same",IF(AND(A121&lt;&gt;C121,D121="same"),"id",IF(B121&lt;&gt;D121,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>72</v>
+        <v>611</v>
       </c>
       <c r="B122" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="C122" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B122,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23410,19 +23179,19 @@
       </c>
       <c r="D122" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A122,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wabash Ave &amp; 16th St</v>
+        <v>same</v>
       </c>
       <c r="E122" t="str">
         <f>IF(AND(D122="same",C122="same"),"missing",IF(B122=D122,"same",IF(AND(A122&lt;&gt;C122,D122="same"),"id",IF(B122&lt;&gt;D122,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>110</v>
+        <v>612</v>
       </c>
       <c r="B123" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="C123" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B123,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23430,19 +23199,19 @@
       </c>
       <c r="D123" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A123,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Dearborn St &amp; Erie St</v>
+        <v>same</v>
       </c>
       <c r="E123" t="str">
         <f>IF(AND(D123="same",C123="same"),"missing",IF(B123=D123,"same",IF(AND(A123&lt;&gt;C123,D123="same"),"id",IF(B123&lt;&gt;D123,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>649</v>
+        <v>613</v>
       </c>
       <c r="B124" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="C124" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B124,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23450,19 +23219,19 @@
       </c>
       <c r="D124" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A124,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Stewart Ave &amp; 63rd St</v>
+        <v>same</v>
       </c>
       <c r="E124" t="str">
         <f>IF(AND(D124="same",C124="same"),"missing",IF(B124=D124,"same",IF(AND(A124&lt;&gt;C124,D124="same"),"id",IF(B124&lt;&gt;D124,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>35</v>
+        <v>613</v>
       </c>
       <c r="B125" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="C125" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B125,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23470,19 +23239,19 @@
       </c>
       <c r="D125" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A125,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Streeter Dr &amp; Grand Ave</v>
+        <v>same</v>
       </c>
       <c r="E125" t="str">
         <f>IF(AND(D125="same",C125="same"),"missing",IF(B125=D125,"same",IF(AND(A125&lt;&gt;C125,D125="same"),"id",IF(B125&lt;&gt;D125,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>19</v>
+        <v>614</v>
       </c>
       <c r="B126" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="C126" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B126,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23490,19 +23259,19 @@
       </c>
       <c r="D126" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A126,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Throop St &amp; Taylor St</v>
+        <v>same</v>
       </c>
       <c r="E126" t="str">
         <f>IF(AND(D126="same",C126="same"),"missing",IF(B126=D126,"same",IF(AND(A126&lt;&gt;C126,D126="same"),"id",IF(B126&lt;&gt;D126,"name"))))</f>
-        <v>name</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>missing</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>363</v>
+        <v>615</v>
       </c>
       <c r="B127" t="s">
-        <v>85</v>
+        <v>129</v>
       </c>
       <c r="C127" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B127,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23519,10 +23288,10 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>408</v>
+        <v>616</v>
       </c>
       <c r="B128" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="C128" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B128,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23530,19 +23299,19 @@
       </c>
       <c r="D128" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A128,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Union Ave &amp; Root St</v>
+        <v>same</v>
       </c>
       <c r="E128" t="str">
         <f>IF(AND(D128="same",C128="same"),"missing",IF(B128=D128,"same",IF(AND(A128&lt;&gt;C128,D128="same"),"id",IF(B128&lt;&gt;D128,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>84</v>
+        <v>617</v>
       </c>
       <c r="B129" t="s">
-        <v>27</v>
+        <v>131</v>
       </c>
       <c r="C129" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B129,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23550,19 +23319,19 @@
       </c>
       <c r="D129" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A129,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Milwaukee Ave &amp; Grand Ave</v>
+        <v>same</v>
       </c>
       <c r="E129" t="str">
         <f>IF(AND(D129="same",C129="same"),"missing",IF(B129=D129,"same",IF(AND(A129&lt;&gt;C129,D129="same"),"id",IF(B129&lt;&gt;D129,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>321</v>
+        <v>618</v>
       </c>
       <c r="B130" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="C130" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B130,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23570,19 +23339,19 @@
       </c>
       <c r="D130" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A130,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wabash Ave &amp; 9th St</v>
+        <v>same</v>
       </c>
       <c r="E130" t="str">
         <f>IF(AND(D130="same",C130="same"),"missing",IF(B130=D130,"same",IF(AND(A130&lt;&gt;C130,D130="same"),"id",IF(B130&lt;&gt;D130,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>72</v>
+        <v>624</v>
       </c>
       <c r="B131" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
       <c r="C131" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B131,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23590,7 +23359,7 @@
       </c>
       <c r="D131" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A131,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wabash Ave &amp; 16th St</v>
+        <v>Dearborn St &amp; Van Buren St</v>
       </c>
       <c r="E131" t="str">
         <f>IF(AND(D131="same",C131="same"),"missing",IF(B131=D131,"same",IF(AND(A131&lt;&gt;C131,D131="same"),"id",IF(B131&lt;&gt;D131,"name"))))</f>
@@ -23599,10 +23368,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>278</v>
+        <v>625</v>
       </c>
       <c r="B132" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="C132" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B132,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23610,7 +23379,7 @@
       </c>
       <c r="D132" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A132,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wallace St &amp; 35th St</v>
+        <v>Dodge Ave &amp; Main St</v>
       </c>
       <c r="E132" t="str">
         <f>IF(AND(D132="same",C132="same"),"missing",IF(B132=D132,"same",IF(AND(A132&lt;&gt;C132,D132="same"),"id",IF(B132&lt;&gt;D132,"name"))))</f>
@@ -23619,10 +23388,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>437</v>
+        <v>627</v>
       </c>
       <c r="B133" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="C133" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B133,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23630,7 +23399,7 @@
       </c>
       <c r="D133" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A133,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Washtenaw Ave &amp; Ogden Ave</v>
+        <v>LaSalle Dr &amp; Huron St</v>
       </c>
       <c r="E133" t="str">
         <f>IF(AND(D133="same",C133="same"),"missing",IF(B133=D133,"same",IF(AND(A133&lt;&gt;C133,D133="same"),"id",IF(B133&lt;&gt;D133,"name"))))</f>
@@ -23639,10 +23408,10 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>437</v>
+        <v>631</v>
       </c>
       <c r="B134" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="C134" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B134,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23650,7 +23419,7 @@
       </c>
       <c r="D134" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A134,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Washtenaw Ave &amp; Ogden Ave</v>
+        <v>Malcolm X College Vaccination Site</v>
       </c>
       <c r="E134" t="str">
         <f>IF(AND(D134="same",C134="same"),"missing",IF(B134=D134,"same",IF(AND(A134&lt;&gt;C134,D134="same"),"id",IF(B134&lt;&gt;D134,"name"))))</f>
@@ -23659,10 +23428,10 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>437</v>
+        <v>635</v>
       </c>
       <c r="B135" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="C135" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B135,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23670,7 +23439,7 @@
       </c>
       <c r="D135" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A135,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Washtenaw Ave &amp; Ogden Ave</v>
+        <v>Fairbanks St &amp; Superior St</v>
       </c>
       <c r="E135" t="str">
         <f>IF(AND(D135="same",C135="same"),"missing",IF(B135=D135,"same",IF(AND(A135&lt;&gt;C135,D135="same"),"id",IF(B135&lt;&gt;D135,"name"))))</f>
@@ -23679,10 +23448,10 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>289</v>
+        <v>636</v>
       </c>
       <c r="B136" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="C136" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B136,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23690,7 +23459,7 @@
       </c>
       <c r="D136" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A136,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wells St &amp; Concord Ln</v>
+        <v>Orleans St &amp; Hubbard St</v>
       </c>
       <c r="E136" t="str">
         <f>IF(AND(D136="same",C136="same"),"missing",IF(B136=D136,"same",IF(AND(A136&lt;&gt;C136,D136="same"),"id",IF(B136&lt;&gt;D136,"name"))))</f>
@@ -23699,10 +23468,10 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>53</v>
+        <v>637</v>
       </c>
       <c r="B137" t="s">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="C137" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B137,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23710,7 +23479,7 @@
       </c>
       <c r="D137" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A137,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wells St &amp; Huron St</v>
+        <v>Wood St &amp; Chicago Ave</v>
       </c>
       <c r="E137" t="str">
         <f>IF(AND(D137="same",C137="same"),"missing",IF(B137=D137,"same",IF(AND(A137&lt;&gt;C137,D137="same"),"id",IF(B137&lt;&gt;D137,"name"))))</f>
@@ -23719,10 +23488,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>132</v>
+        <v>638</v>
       </c>
       <c r="B138" t="s">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="C138" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B138,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23730,7 +23499,7 @@
       </c>
       <c r="D138" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A138,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wentworth Ave &amp; 24th St Temp</v>
+        <v>Clinton St &amp; Jackson Blvd</v>
       </c>
       <c r="E138" t="str">
         <f>IF(AND(D138="same",C138="same"),"missing",IF(B138=D138,"same",IF(AND(A138&lt;&gt;C138,D138="same"),"id",IF(B138&lt;&gt;D138,"name"))))</f>
@@ -23739,10 +23508,10 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>120</v>
+        <v>643</v>
       </c>
       <c r="B139" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="C139" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B139,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23750,7 +23519,7 @@
       </c>
       <c r="D139" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A139,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wentworth Ave &amp; Cermak Rd</v>
+        <v>Smith Park</v>
       </c>
       <c r="E139" t="str">
         <f>IF(AND(D139="same",C139="same"),"missing",IF(B139=D139,"same",IF(AND(A139&lt;&gt;C139,D139="same"),"id",IF(B139&lt;&gt;D139,"name"))))</f>
@@ -23759,10 +23528,10 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>120</v>
+        <v>644</v>
       </c>
       <c r="B140" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="C140" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B140,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23770,7 +23539,7 @@
       </c>
       <c r="D140" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A140,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wentworth Ave &amp; Cermak Rd</v>
+        <v>Western Ave &amp; Fillmore St</v>
       </c>
       <c r="E140" t="str">
         <f>IF(AND(D140="same",C140="same"),"missing",IF(B140=D140,"same",IF(AND(A140&lt;&gt;C140,D140="same"),"id",IF(B140&lt;&gt;D140,"name"))))</f>
@@ -23779,10 +23548,10 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>446</v>
+        <v>645</v>
       </c>
       <c r="B141" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="C141" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B141,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23790,7 +23559,7 @@
       </c>
       <c r="D141" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A141,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Western &amp; 28th - Velasquez Institute Vaccination Site</v>
+        <v>Archer Damen Ave &amp; 37th St</v>
       </c>
       <c r="E141" t="str">
         <f>IF(AND(D141="same",C141="same"),"missing",IF(B141=D141,"same",IF(AND(A141&lt;&gt;C141,D141="same"),"id",IF(B141&lt;&gt;D141,"name"))))</f>
@@ -23799,10 +23568,10 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>644</v>
+        <v>649</v>
       </c>
       <c r="B142" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C142" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B142,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23810,19 +23579,19 @@
       </c>
       <c r="D142" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A142,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Western Ave &amp; Fillmore St</v>
+        <v>Stewart Ave &amp; 63rd St</v>
       </c>
       <c r="E142" t="str">
         <f>IF(AND(D142="same",C142="same"),"missing",IF(B142=D142,"same",IF(AND(A142&lt;&gt;C142,D142="same"),"id",IF(B142&lt;&gt;D142,"name"))))</f>
         <v>name</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>613</v>
+        <v>650</v>
       </c>
       <c r="B143" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="C143" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B143,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23830,23 +23599,23 @@
       </c>
       <c r="D143" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A143,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>Eggleston Ave &amp; 69th St</v>
       </c>
       <c r="E143" t="str">
         <f>IF(AND(D143="same",C143="same"),"missing",IF(B143=D143,"same",IF(AND(A143&lt;&gt;C143,D143="same"),"id",IF(B143&lt;&gt;D143,"name"))))</f>
-        <v>missing</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>name</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>613</v>
+        <v>651</v>
       </c>
       <c r="B144" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="C144" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B144,0),Stations!$B:$D,2,FALSE),"same")</f>
-        <v>same</v>
+        <v>674</v>
       </c>
       <c r="D144" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A144,0),Stations!$A:$B,2,FALSE),"same")</f>
@@ -23854,15 +23623,15 @@
       </c>
       <c r="E144" t="str">
         <f>IF(AND(D144="same",C144="same"),"missing",IF(B144=D144,"same",IF(AND(A144&lt;&gt;C144,D144="same"),"id",IF(B144&lt;&gt;D144,"name"))))</f>
-        <v>missing</v>
+        <v>id</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>238</v>
+        <v>654</v>
       </c>
       <c r="B145" t="s">
-        <v>57</v>
+        <v>147</v>
       </c>
       <c r="C145" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B145,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23870,7 +23639,7 @@
       </c>
       <c r="D145" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A145,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wolcott Ravenswood Ave &amp; Montrose Ave</v>
+        <v>Racine Ave &amp; Washington Blvd</v>
       </c>
       <c r="E145" t="str">
         <f>IF(AND(D145="same",C145="same"),"missing",IF(B145=D145,"same",IF(AND(A145&lt;&gt;C145,D145="same"),"id",IF(B145&lt;&gt;D145,"name"))))</f>
@@ -23879,10 +23648,10 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>637</v>
+        <v>656</v>
       </c>
       <c r="B146" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="C146" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B146,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23890,7 +23659,7 @@
       </c>
       <c r="D146" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A146,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wood St &amp; Chicago Ave</v>
+        <v>Damen Ave &amp; Walnut Lake St</v>
       </c>
       <c r="E146" t="str">
         <f>IF(AND(D146="same",C146="same"),"missing",IF(B146=D146,"same",IF(AND(A146&lt;&gt;C146,D146="same"),"id",IF(B146&lt;&gt;D146,"name"))))</f>
@@ -23899,10 +23668,10 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>17</v>
+        <v>658</v>
       </c>
       <c r="B147" t="s">
-        <v>8</v>
+        <v>149</v>
       </c>
       <c r="C147" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B147,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23910,7 +23679,7 @@
       </c>
       <c r="D147" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A147,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Honore St &amp; Division St</v>
+        <v>Leavitt St &amp; Division St</v>
       </c>
       <c r="E147" t="str">
         <f>IF(AND(D147="same",C147="same"),"missing",IF(B147=D147,"same",IF(AND(A147&lt;&gt;C147,D147="same"),"id",IF(B147&lt;&gt;D147,"name"))))</f>
@@ -23919,10 +23688,10 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>285</v>
+        <v>664</v>
       </c>
       <c r="B148" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
       <c r="C148" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B148,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23930,7 +23699,7 @@
       </c>
       <c r="D148" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A148,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wood St &amp; Hubbard St</v>
+        <v>Leavitt St &amp; Belmont Ave</v>
       </c>
       <c r="E148" t="str">
         <f>IF(AND(D148="same",C148="same"),"missing",IF(B148=D148,"same",IF(AND(A148&lt;&gt;C148,D148="same"),"id",IF(B148&lt;&gt;D148,"name"))))</f>
@@ -23939,10 +23708,10 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>16</v>
+        <v>669</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>151</v>
       </c>
       <c r="C149" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B149,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23950,19 +23719,19 @@
       </c>
       <c r="D149" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A149,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Paulina Ave &amp; North Ave</v>
+        <v>same</v>
       </c>
       <c r="E149" t="str">
         <f>IF(AND(D149="same",C149="same"),"missing",IF(B149=D149,"same",IF(AND(A149&lt;&gt;C149,D149="same"),"id",IF(B149&lt;&gt;D149,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>317</v>
+        <v>671</v>
       </c>
       <c r="B150" t="s">
-        <v>73</v>
+        <v>152</v>
       </c>
       <c r="C150" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(B150,0),Stations!$B:$D,2,FALSE),"same")</f>
@@ -23970,48 +23739,43 @@
       </c>
       <c r="D150" t="str">
         <f>_xlfn.IFNA(VLOOKUP(TEXT(A150,0),Stations!$A:$B,2,FALSE),"same")</f>
-        <v>Wood St &amp; Taylor St Temp</v>
+        <v>same</v>
       </c>
       <c r="E150" t="str">
         <f>IF(AND(D150="same",C150="same"),"missing",IF(B150=D150,"same",IF(AND(A150&lt;&gt;C150,D150="same"),"id",IF(B150&lt;&gt;D150,"name"))))</f>
-        <v>name</v>
+        <v>missing</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E150">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="name"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:E150" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E150">
-      <sortCondition ref="B1:B150"/>
+      <sortCondition ref="A1:A150"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="missing">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="missing">
       <formula>NOT(ISERROR(SEARCH("missing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="same">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="same">
       <formula>NOT(ISERROR(SEARCH("same",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="name">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="name">
       <formula>NOT(ISERROR(SEARCH("name",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="missing">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="missing">
       <formula>NOT(ISERROR(SEARCH("missing",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="id">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="id">
       <formula>NOT(ISERROR(SEARCH("id",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="none">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="none">
       <formula>NOT(ISERROR(SEARCH("none",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="same">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="same">
       <formula>NOT(ISERROR(SEARCH("same",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24020,7 +23784,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -57607,7 +57371,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1291"/>
+  <autoFilter ref="A1:H1291" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>